<commit_message>
actualizacion de los doc's mala ortografia
el plan summary no estaba bien generado perdon
</commit_message>
<xml_diff>
--- a/Documentación/Psp's/Tania/Clase BD_ControlEscolar/Plan Sumary.xlsx
+++ b/Documentación/Psp's/Tania/Clase BD_ControlEscolar/Plan Sumary.xlsx
@@ -15,7 +15,7 @@
     <sheet name="excel" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="excel" localSheetId="0">excel!$A$1:$D$29</definedName>
+    <definedName name="excel" localSheetId="0">excel!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -23,14 +23,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\TaniaEsparza\Desktop\Clase BD_ControlEscolar\excel.iqy" name="excel" type="4" refreshedVersion="5" background="1" saveData="1">
-    <webPr consecutive="1" xl2000="1" url="http://localhost:2468/reports/form2html.class?uri=%2FProject%2FCodificacion%2BBD%2BControl%2BEscolar%2FPSP2%2E1%2F%2Fcms%2Fpsp2%2E1%2Fsummary%3Fframe%3Dcontent%26section%3D102&amp;EXPORT=excel" htmlFormat="all"/>
+  <connection id="1" odcFile="C:\Users\TaniaEsparza\Downloads\excel.iqy" name="excel" type="4" refreshedVersion="5" background="1" saveData="1">
+    <webPr consecutive="1" xl2000="1" url="http://localhost:2468/reports/form2html.class?uri=%2FProject%2FCodificacion%2BBD%2BControl%2BEscolar%2FPSP2%2E1%2F%2Fcms%2Fpsp2%2E1%2Fsummary%3Fframe%3Dcontent%26section%3D105&amp;EXPORT=excel" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>/Project/Codificacion BD Control Escolar/PSP2.1</t>
   </si>
@@ -38,10 +38,7 @@
     <t>PSP2.1 Project Plan Summary</t>
   </si>
   <si>
-    <t>Overall Metrics</t>
-  </si>
-  <si>
-    <t>Summary</t>
+    <t>Program Size</t>
   </si>
   <si>
     <t>Plan</t>
@@ -53,61 +50,52 @@
     <t>To Date</t>
   </si>
   <si>
-    <t>Size/Hour</t>
-  </si>
-  <si>
-    <t>Planned Time</t>
-  </si>
-  <si>
-    <t>Actual Time</t>
-  </si>
-  <si>
-    <t>CPI (Cost-Performance Index)</t>
-  </si>
-  <si>
-    <t>% Reuse</t>
-  </si>
-  <si>
-    <t>% New Reusable</t>
-  </si>
-  <si>
-    <t>Test Defects/KLOC or equivalent</t>
-  </si>
-  <si>
-    <t>Total Defects/KLOC or equivalent</t>
-  </si>
-  <si>
-    <t>Yield %</t>
-  </si>
-  <si>
-    <t>Code Review Rate</t>
-  </si>
-  <si>
-    <t>% Appraisal COQ</t>
-  </si>
-  <si>
-    <t>% Failure COQ</t>
-  </si>
-  <si>
-    <t>COQ A/F Ratio</t>
-  </si>
-  <si>
-    <t>PQI</t>
+    <t>Base (B)</t>
+  </si>
+  <si>
+    <t>Deleted (D)</t>
+  </si>
+  <si>
+    <t>Modified (M)</t>
+  </si>
+  <si>
+    <t>Added (A)</t>
+  </si>
+  <si>
+    <t>Reused (R)</t>
+  </si>
+  <si>
+    <t>Added and Modified (A+M)</t>
+  </si>
+  <si>
+    <t>Total Size (T)</t>
+  </si>
+  <si>
+    <t>Total New Reusable</t>
+  </si>
+  <si>
+    <t>Estimated Proxy Size (E)</t>
+  </si>
+  <si>
+    <t>Upper Prediction Interval (70%)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Lower Prediction Interval (70%)</t>
   </si>
   <si>
     <t>Adapted from "PSP Materials," copyright © 2006 Carnegie Mellon University. Used by permission.</t>
   </si>
   <si>
-    <t>Report generated at 9:35 AM on Nov 13, 2018</t>
+    <t>Report generated at 8:40 PM on Nov 14, 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[h]\:mm"/>
-  </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,7 +629,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -662,30 +650,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1019,17 +989,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1058,221 +1026,177 @@
       <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="C8" s="7">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="D8" s="7">
-        <v>40.299999999999997</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10">
-        <v>0.14166666666666666</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0.14166666666666666</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7">
-        <v>1.18</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>163</v>
+      </c>
+      <c r="C11" s="8">
+        <v>161</v>
+      </c>
+      <c r="D11" s="8">
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="B13" s="7">
+        <v>163</v>
+      </c>
+      <c r="C13" s="8">
+        <v>161</v>
+      </c>
+      <c r="D13" s="8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
-        <v>0</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="7">
+        <v>163</v>
+      </c>
+      <c r="C14" s="8">
+        <v>161</v>
+      </c>
+      <c r="D14" s="8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8">
-        <v>5</v>
-      </c>
-      <c r="C14" s="7">
-        <v>14.6</v>
-      </c>
-      <c r="D14" s="7">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8">
-        <v>65</v>
-      </c>
-      <c r="C15" s="7">
-        <v>36.5</v>
-      </c>
-      <c r="D15" s="7">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B16" s="7">
+        <v>163</v>
+      </c>
+      <c r="C16" s="8">
+        <v>161</v>
+      </c>
+      <c r="D16" s="8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="13">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="C16" s="12">
-        <v>0.6</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8">
-        <v>326</v>
-      </c>
-      <c r="C17" s="7">
-        <v>329</v>
-      </c>
-      <c r="D17" s="7">
-        <v>329</v>
-      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
-        <v>0.25</v>
-      </c>
-      <c r="C18" s="15">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0.21099999999999999</v>
-      </c>
+      <c r="B18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="C19" s="15">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="D19" s="15">
-        <v>0.13700000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" s="8">
-        <v>1.67</v>
-      </c>
-      <c r="C20" s="7">
-        <v>1.54</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="8">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0.22</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>